<commit_message>
Various changes from adding more tests to redoing data1-3.xlsx
</commit_message>
<xml_diff>
--- a/data3.xlsx
+++ b/data3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itapp\PycharmProjects\WLalgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621596EC-2E47-4670-905C-28D59A5B828C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4B9BF0-E6AB-4A5E-82E3-10DDB0B68798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,6 +156,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>data!$A$1:$A$148</c:f>
@@ -1822,10 +1837,10 @@
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>